<commit_message>
Crear Paquetes Dao y Service, crear interfaces e implementaciones de cada service
</commit_message>
<xml_diff>
--- a/compiladores-laboratorio1/src/main/resources/Hoja.xlsx
+++ b/compiladores-laboratorio1/src/main/resources/Hoja.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Libro" sheetId="2" r:id="rId1"/>
@@ -594,7 +594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -906,7 +906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>